<commit_message>
new comparison files for (0,0,0)
</commit_message>
<xml_diff>
--- a/output/predicted_trajectoriesX.xlsx
+++ b/output/predicted_trajectoriesX.xlsx
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1482.763321644422</v>
+        <v>1831.591157525936</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>0.03333333333333333</v>
       </c>
       <c r="B3" t="n">
-        <v>2295.943700484928</v>
+        <v>2900.686774403619</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>0.06666666666666667</v>
       </c>
       <c r="B4" t="n">
-        <v>3590.303594718952</v>
+        <v>3895.74006538886</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>0.1</v>
       </c>
       <c r="B5" t="n">
-        <v>4123.98618705811</v>
+        <v>4359.462888536614</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>0.1333333333333333</v>
       </c>
       <c r="B6" t="n">
-        <v>4632.454430432118</v>
+        <v>4908.677389009084</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>0.1666666666666667</v>
       </c>
       <c r="B7" t="n">
-        <v>5078.195575588124</v>
+        <v>5486.642319586107</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>0.2</v>
       </c>
       <c r="B8" t="n">
-        <v>5461.220293632206</v>
+        <v>5700.138037599012</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>0.2333333333333333</v>
       </c>
       <c r="B9" t="n">
-        <v>5874.652607844609</v>
+        <v>6001.457960867561</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>0.2666666666666667</v>
       </c>
       <c r="B10" t="n">
-        <v>6332.620533391886</v>
+        <v>6347.371853381838</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>0.3</v>
       </c>
       <c r="B11" t="n">
-        <v>6439.039675104013</v>
+        <v>6511.84542830972</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="B12" t="n">
-        <v>6500.640313616914</v>
+        <v>6794.667971583616</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>0.3666666666666666</v>
       </c>
       <c r="B13" t="n">
-        <v>6978.173515253572</v>
+        <v>6987.925687287144</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>0.4</v>
       </c>
       <c r="B14" t="n">
-        <v>7043.000656147563</v>
+        <v>7074.915236817072</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>0.4333333333333333</v>
       </c>
       <c r="B15" t="n">
-        <v>7228.234605111224</v>
+        <v>7302.369183577823</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>0.4666666666666667</v>
       </c>
       <c r="B16" t="n">
-        <v>7389.685645756293</v>
+        <v>7425.296298002776</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>0.5</v>
       </c>
       <c r="B17" t="n">
-        <v>7618.50920885412</v>
+        <v>7639.665539629861</v>
       </c>
     </row>
     <row r="18">
@@ -578,7 +578,7 @@
         <v>0.5333333333333333</v>
       </c>
       <c r="B18" t="n">
-        <v>7671.53378163277</v>
+        <v>7705.27926169254</v>
       </c>
     </row>
     <row r="19">
@@ -586,7 +586,7 @@
         <v>0.5666666666666667</v>
       </c>
       <c r="B19" t="n">
-        <v>7786.266272578909</v>
+        <v>7895.640957707441</v>
       </c>
     </row>
     <row r="20">
@@ -594,7 +594,7 @@
         <v>0.6</v>
       </c>
       <c r="B20" t="n">
-        <v>7932.234214873523</v>
+        <v>7998.670052572564</v>
       </c>
     </row>
     <row r="21">
@@ -602,7 +602,7 @@
         <v>0.6333333333333333</v>
       </c>
       <c r="B21" t="n">
-        <v>7989.492511114588</v>
+        <v>8037.150975487283</v>
       </c>
     </row>
     <row r="22">
@@ -610,7 +610,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>8096.400578975315</v>
+        <v>8150.445646074456</v>
       </c>
     </row>
     <row r="23">
@@ -618,7 +618,7 @@
         <v>0.7</v>
       </c>
       <c r="B23" t="n">
-        <v>8196.711765146063</v>
+        <v>8241.785704796668</v>
       </c>
     </row>
     <row r="24">
@@ -626,7 +626,7 @@
         <v>0.7333333333333333</v>
       </c>
       <c r="B24" t="n">
-        <v>8229.453751420204</v>
+        <v>8273.790333035993</v>
       </c>
     </row>
     <row r="25">
@@ -634,7 +634,7 @@
         <v>0.7666666666666666</v>
       </c>
       <c r="B25" t="n">
-        <v>8239.870370291952</v>
+        <v>8280.59494368448</v>
       </c>
     </row>
     <row r="26">
@@ -642,7 +642,7 @@
         <v>0.8</v>
       </c>
       <c r="B26" t="n">
-        <v>8239.870370291952</v>
+        <v>8292.317813205944</v>
       </c>
     </row>
     <row r="27">
@@ -650,7 +650,7 @@
         <v>0.8333333333333334</v>
       </c>
       <c r="B27" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="28">
@@ -658,7 +658,7 @@
         <v>0.8666666666666667</v>
       </c>
       <c r="B28" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="29">
@@ -666,7 +666,7 @@
         <v>0.9</v>
       </c>
       <c r="B29" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +674,7 @@
         <v>0.9333333333333333</v>
       </c>
       <c r="B30" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="31">
@@ -682,7 +682,7 @@
         <v>0.9666666666666667</v>
       </c>
       <c r="B31" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="32">
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="33">
@@ -698,7 +698,7 @@
         <v>1.033333333333333</v>
       </c>
       <c r="B33" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="34">
@@ -706,7 +706,7 @@
         <v>1.066666666666667</v>
       </c>
       <c r="B34" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="35">
@@ -714,7 +714,7 @@
         <v>1.1</v>
       </c>
       <c r="B35" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="36">
@@ -722,7 +722,7 @@
         <v>1.133333333333333</v>
       </c>
       <c r="B36" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="37">
@@ -730,7 +730,7 @@
         <v>1.166666666666667</v>
       </c>
       <c r="B37" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="38">
@@ -738,7 +738,7 @@
         <v>1.2</v>
       </c>
       <c r="B38" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="39">
@@ -746,7 +746,7 @@
         <v>1.233333333333333</v>
       </c>
       <c r="B39" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +754,7 @@
         <v>1.266666666666667</v>
       </c>
       <c r="B40" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="41">
@@ -762,7 +762,7 @@
         <v>1.3</v>
       </c>
       <c r="B41" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="42">
@@ -770,7 +770,7 @@
         <v>1.333333333333333</v>
       </c>
       <c r="B42" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="43">
@@ -778,7 +778,7 @@
         <v>1.366666666666667</v>
       </c>
       <c r="B43" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="44">
@@ -786,7 +786,7 @@
         <v>1.4</v>
       </c>
       <c r="B44" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="45">
@@ -794,7 +794,7 @@
         <v>1.433333333333333</v>
       </c>
       <c r="B45" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="46">
@@ -802,7 +802,7 @@
         <v>1.466666666666667</v>
       </c>
       <c r="B46" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="47">
@@ -810,7 +810,7 @@
         <v>1.5</v>
       </c>
       <c r="B47" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="48">
@@ -818,7 +818,7 @@
         <v>1.533333333333333</v>
       </c>
       <c r="B48" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="49">
@@ -826,7 +826,7 @@
         <v>1.566666666666667</v>
       </c>
       <c r="B49" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="50">
@@ -834,7 +834,7 @@
         <v>1.6</v>
       </c>
       <c r="B50" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="51">
@@ -842,7 +842,7 @@
         <v>1.633333333333333</v>
       </c>
       <c r="B51" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="52">
@@ -850,7 +850,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="B52" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="53">
@@ -858,7 +858,7 @@
         <v>1.7</v>
       </c>
       <c r="B53" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="54">
@@ -866,7 +866,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="B54" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="55">
@@ -874,7 +874,7 @@
         <v>1.766666666666667</v>
       </c>
       <c r="B55" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="56">
@@ -882,7 +882,7 @@
         <v>1.8</v>
       </c>
       <c r="B56" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="57">
@@ -890,7 +890,7 @@
         <v>1.833333333333333</v>
       </c>
       <c r="B57" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="58">
@@ -898,7 +898,7 @@
         <v>1.866666666666667</v>
       </c>
       <c r="B58" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="59">
@@ -906,7 +906,7 @@
         <v>1.9</v>
       </c>
       <c r="B59" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="60">
@@ -914,7 +914,7 @@
         <v>1.933333333333333</v>
       </c>
       <c r="B60" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="61">
@@ -922,7 +922,7 @@
         <v>1.966666666666667</v>
       </c>
       <c r="B61" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
     <row r="62">
@@ -930,7 +930,7 @@
         <v>2</v>
       </c>
       <c r="B62" t="n">
-        <v>8239.870370297313</v>
+        <v>8293.00593833287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed 2 versions of robot code w sample trajectory data
</commit_message>
<xml_diff>
--- a/output/predicted_trajectoriesX.xlsx
+++ b/output/predicted_trajectoriesX.xlsx
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1831.591157525936</v>
+        <v>1934.919849777034</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>0.03333333333333333</v>
       </c>
       <c r="B3" t="n">
-        <v>2900.686774403619</v>
+        <v>2988.576002886201</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>0.06666666666666667</v>
       </c>
       <c r="B4" t="n">
-        <v>3895.74006538886</v>
+        <v>4166.878890431921</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>0.1</v>
       </c>
       <c r="B5" t="n">
-        <v>4359.462888536614</v>
+        <v>4696.545507286738</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>0.1333333333333333</v>
       </c>
       <c r="B6" t="n">
-        <v>4908.677389009084</v>
+        <v>5102.612874897974</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>0.1666666666666667</v>
       </c>
       <c r="B7" t="n">
-        <v>5486.642319586107</v>
+        <v>5936.571654466956</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>0.2</v>
       </c>
       <c r="B8" t="n">
-        <v>5700.138037599012</v>
+        <v>6231.96760524919</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>0.2333333333333333</v>
       </c>
       <c r="B9" t="n">
-        <v>6001.457960867561</v>
+        <v>6409.291201575541</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>0.2666666666666667</v>
       </c>
       <c r="B10" t="n">
-        <v>6347.371853381838</v>
+        <v>6750.207609667235</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>0.3</v>
       </c>
       <c r="B11" t="n">
-        <v>6511.84542830972</v>
+        <v>6953.238624305999</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="B12" t="n">
-        <v>6794.667971583616</v>
+        <v>7072.01671505661</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>0.3666666666666666</v>
       </c>
       <c r="B13" t="n">
-        <v>6987.925687287144</v>
+        <v>7408.09351793669</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>0.4</v>
       </c>
       <c r="B14" t="n">
-        <v>7074.915236817072</v>
+        <v>7560.113295091199</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>0.4333333333333333</v>
       </c>
       <c r="B15" t="n">
-        <v>7302.369183577823</v>
+        <v>7672.016297393805</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>0.4666666666666667</v>
       </c>
       <c r="B16" t="n">
-        <v>7425.296298002776</v>
+        <v>7873.389020378461</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>0.5</v>
       </c>
       <c r="B17" t="n">
-        <v>7639.665539629861</v>
+        <v>8008.031782703364</v>
       </c>
     </row>
     <row r="18">
@@ -578,7 +578,7 @@
         <v>0.5333333333333333</v>
       </c>
       <c r="B18" t="n">
-        <v>7705.27926169254</v>
+        <v>8095.19391187989</v>
       </c>
     </row>
     <row r="19">
@@ -586,7 +586,7 @@
         <v>0.5666666666666667</v>
       </c>
       <c r="B19" t="n">
-        <v>7895.640957707441</v>
+        <v>8167.362054571519</v>
       </c>
     </row>
     <row r="20">
@@ -594,7 +594,7 @@
         <v>0.6</v>
       </c>
       <c r="B20" t="n">
-        <v>7998.670052572564</v>
+        <v>8341.539911358934</v>
       </c>
     </row>
     <row r="21">
@@ -602,7 +602,7 @@
         <v>0.6333333333333333</v>
       </c>
       <c r="B21" t="n">
-        <v>8037.150975487283</v>
+        <v>8390.094114595906</v>
       </c>
     </row>
     <row r="22">
@@ -610,7 +610,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>8150.445646074456</v>
+        <v>8453.696374182065</v>
       </c>
     </row>
     <row r="23">
@@ -618,7 +618,7 @@
         <v>0.7</v>
       </c>
       <c r="B23" t="n">
-        <v>8241.785704796668</v>
+        <v>8457.615102224545</v>
       </c>
     </row>
     <row r="24">
@@ -626,7 +626,7 @@
         <v>0.7333333333333333</v>
       </c>
       <c r="B24" t="n">
-        <v>8273.790333035993</v>
+        <v>8460.208531760383</v>
       </c>
     </row>
     <row r="25">
@@ -634,7 +634,7 @@
         <v>0.7666666666666666</v>
       </c>
       <c r="B25" t="n">
-        <v>8280.59494368448</v>
+        <v>8467.217522703546</v>
       </c>
     </row>
     <row r="26">
@@ -642,7 +642,7 @@
         <v>0.8</v>
       </c>
       <c r="B26" t="n">
-        <v>8292.317813205944</v>
+        <v>8460.199749823316</v>
       </c>
     </row>
     <row r="27">
@@ -650,7 +650,7 @@
         <v>0.8333333333333334</v>
       </c>
       <c r="B27" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="28">
@@ -658,7 +658,7 @@
         <v>0.8666666666666667</v>
       </c>
       <c r="B28" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="29">
@@ -666,7 +666,7 @@
         <v>0.9</v>
       </c>
       <c r="B29" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +674,7 @@
         <v>0.9333333333333333</v>
       </c>
       <c r="B30" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="31">
@@ -682,7 +682,7 @@
         <v>0.9666666666666667</v>
       </c>
       <c r="B31" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="32">
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="33">
@@ -698,7 +698,7 @@
         <v>1.033333333333333</v>
       </c>
       <c r="B33" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="34">
@@ -706,7 +706,7 @@
         <v>1.066666666666667</v>
       </c>
       <c r="B34" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="35">
@@ -714,7 +714,7 @@
         <v>1.1</v>
       </c>
       <c r="B35" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="36">
@@ -722,7 +722,7 @@
         <v>1.133333333333333</v>
       </c>
       <c r="B36" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="37">
@@ -730,7 +730,7 @@
         <v>1.166666666666667</v>
       </c>
       <c r="B37" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="38">
@@ -738,7 +738,7 @@
         <v>1.2</v>
       </c>
       <c r="B38" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="39">
@@ -746,7 +746,7 @@
         <v>1.233333333333333</v>
       </c>
       <c r="B39" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +754,7 @@
         <v>1.266666666666667</v>
       </c>
       <c r="B40" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="41">
@@ -762,7 +762,7 @@
         <v>1.3</v>
       </c>
       <c r="B41" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="42">
@@ -770,7 +770,7 @@
         <v>1.333333333333333</v>
       </c>
       <c r="B42" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="43">
@@ -778,7 +778,7 @@
         <v>1.366666666666667</v>
       </c>
       <c r="B43" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="44">
@@ -786,7 +786,7 @@
         <v>1.4</v>
       </c>
       <c r="B44" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="45">
@@ -794,7 +794,7 @@
         <v>1.433333333333333</v>
       </c>
       <c r="B45" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="46">
@@ -802,7 +802,7 @@
         <v>1.466666666666667</v>
       </c>
       <c r="B46" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="47">
@@ -810,7 +810,7 @@
         <v>1.5</v>
       </c>
       <c r="B47" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="48">
@@ -818,7 +818,7 @@
         <v>1.533333333333333</v>
       </c>
       <c r="B48" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="49">
@@ -826,7 +826,7 @@
         <v>1.566666666666667</v>
       </c>
       <c r="B49" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="50">
@@ -834,7 +834,7 @@
         <v>1.6</v>
       </c>
       <c r="B50" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="51">
@@ -842,7 +842,7 @@
         <v>1.633333333333333</v>
       </c>
       <c r="B51" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="52">
@@ -850,7 +850,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="B52" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="53">
@@ -858,7 +858,7 @@
         <v>1.7</v>
       </c>
       <c r="B53" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="54">
@@ -866,7 +866,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="B54" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="55">
@@ -874,7 +874,7 @@
         <v>1.766666666666667</v>
       </c>
       <c r="B55" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="56">
@@ -882,7 +882,7 @@
         <v>1.8</v>
       </c>
       <c r="B56" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="57">
@@ -890,7 +890,7 @@
         <v>1.833333333333333</v>
       </c>
       <c r="B57" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="58">
@@ -898,7 +898,7 @@
         <v>1.866666666666667</v>
       </c>
       <c r="B58" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="59">
@@ -906,7 +906,7 @@
         <v>1.9</v>
       </c>
       <c r="B59" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="60">
@@ -914,7 +914,7 @@
         <v>1.933333333333333</v>
       </c>
       <c r="B60" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="61">
@@ -922,7 +922,7 @@
         <v>1.966666666666667</v>
       </c>
       <c r="B61" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
     <row r="62">
@@ -930,7 +930,7 @@
         <v>2</v>
       </c>
       <c r="B62" t="n">
-        <v>8293.00593833287</v>
+        <v>8460.308567009597</v>
       </c>
     </row>
   </sheetData>

</xml_diff>